<commit_message>
Preparation of databases for screening and analysis (standarize variable names, delete inadecuate values...)
</commit_message>
<xml_diff>
--- a/data/Emergence.xlsx
+++ b/data/Emergence.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://irtacat-my.sharepoint.com/personal/alejandro_munoz_irta_cat/Documents/Documentos/Exclusion-Lisso-Analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD5D3B9D-C9A0-4494-9A7A-86FE35EA150D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{FD5D3B9D-C9A0-4494-9A7A-86FE35EA150D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423C4C98-782B-4E87-B13D-6C031C89A355}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CB3F75C1-EA4D-41FB-801C-C1811436CE28}"/>
+    <workbookView xWindow="28680" yWindow="-7515" windowWidth="29040" windowHeight="15720" xr2:uid="{CB3F75C1-EA4D-41FB-801C-C1811436CE28}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trampas emergencia" sheetId="1" r:id="rId1"/>
+    <sheet name="Emergence traps" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Trampas emergencia'!$L$148:$L$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Emergence traps'!$L$148:$L$148</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,25 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="26">
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>ID Parcela</t>
-  </si>
-  <si>
-    <t>Tratamiento</t>
-  </si>
-  <si>
-    <t>Taxon</t>
-  </si>
-  <si>
-    <t>Abundancia</t>
-  </si>
-  <si>
-    <t>Observaciones</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="20">
   <si>
     <t>BE</t>
   </si>
@@ -68,28 +50,13 @@
     <t>S. fonscolombii</t>
   </si>
   <si>
-    <t>2FC</t>
-  </si>
-  <si>
     <t>FC</t>
-  </si>
-  <si>
-    <t>2FE</t>
-  </si>
-  <si>
-    <t>2BE</t>
   </si>
   <si>
     <t>FE</t>
   </si>
   <si>
-    <t>3BE</t>
-  </si>
-  <si>
     <t>L. oryzophilus</t>
-  </si>
-  <si>
-    <t>4BE</t>
   </si>
   <si>
     <t>FO</t>
@@ -104,9 +71,6 @@
     <t>Aeshnidae</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Vacio</t>
   </si>
   <si>
@@ -117,6 +81,24 @@
   </si>
   <si>
     <t>Vacio, hay pequeña abertura en el triangulo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Taxa</t>
+  </si>
+  <si>
+    <t>Abundance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Treatment</t>
   </si>
 </sst>
 </file>
@@ -303,12 +285,12 @@
     <sortCondition ref="D2:D181"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1D7CD550-C881-4025-B141-32184CAE97E3}" name="Fecha" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{704ADF05-4B18-4A83-AC2A-89BF3B34B753}" name="ID Parcela" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{ED1D907E-3B90-4555-AF71-5A359B4A5868}" name="Tratamiento" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{67C115F7-0860-4847-A729-053FF1CF19D2}" name="Taxon" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A8D949CF-4F2C-492B-88FC-90D60FCCDD67}" name="Abundancia" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{1918495C-E796-4AFC-B80C-0B7A55E86023}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1D7CD550-C881-4025-B141-32184CAE97E3}" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{704ADF05-4B18-4A83-AC2A-89BF3B34B753}" name="Field" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{ED1D907E-3B90-4555-AF71-5A359B4A5868}" name="Treatment" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{67C115F7-0860-4847-A729-053FF1CF19D2}" name="Taxa" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A8D949CF-4F2C-492B-88FC-90D60FCCDD67}" name="Abundance" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1918495C-E796-4AFC-B80C-0B7A55E86023}" name="Observations" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -611,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B505B8-28D2-43BF-8D9D-5BF701E8C9C4}">
-  <dimension ref="A1:I181"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:D130"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -628,27 +610,27 @@
     <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45838</v>
       </c>
@@ -656,16 +638,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45838</v>
       </c>
@@ -673,22 +655,17 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="H3" s="2">
-        <v>45894</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45838</v>
       </c>
@@ -696,22 +673,17 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>104</v>
       </c>
-      <c r="H4" s="2">
-        <v>45894</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45838</v>
       </c>
@@ -719,22 +691,17 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="H5" s="2">
-        <v>45894</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45838</v>
       </c>
@@ -742,22 +709,17 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>172</v>
       </c>
-      <c r="H6" s="2">
-        <v>45894</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45838</v>
       </c>
@@ -765,22 +727,17 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="H7" s="2">
-        <v>45894</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45838</v>
       </c>
@@ -788,16 +745,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45838</v>
       </c>
@@ -805,16 +762,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45838</v>
       </c>
@@ -822,16 +779,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>896</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45838</v>
       </c>
@@ -839,16 +796,16 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45838</v>
       </c>
@@ -856,16 +813,16 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45838</v>
       </c>
@@ -873,16 +830,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45838</v>
       </c>
@@ -890,16 +847,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>572</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45838</v>
       </c>
@@ -907,16 +864,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45838</v>
       </c>
@@ -924,10 +881,10 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>772</v>
@@ -941,10 +898,10 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -958,10 +915,10 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>101</v>
@@ -975,10 +932,10 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <v>5</v>
@@ -992,10 +949,10 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>348</v>
@@ -1009,10 +966,10 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>292</v>
@@ -1026,10 +983,10 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -1043,10 +1000,10 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>101</v>
@@ -1060,10 +1017,10 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1077,10 +1034,10 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1094,10 +1051,10 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>91</v>
@@ -1111,10 +1068,10 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1128,10 +1085,10 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>352</v>
@@ -1145,10 +1102,10 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E29">
         <v>160</v>
@@ -1162,10 +1119,10 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>150</v>
@@ -1179,10 +1136,10 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>324</v>
@@ -1196,10 +1153,10 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>186</v>
@@ -1213,16 +1170,16 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E33">
         <v>36</v>
       </c>
       <c r="F33" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1233,10 +1190,10 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>258</v>
@@ -1250,10 +1207,10 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>23</v>
@@ -1267,10 +1224,10 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E36">
         <v>14</v>
@@ -1284,10 +1241,10 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1301,10 +1258,10 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>57</v>
@@ -1318,10 +1275,10 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E39">
         <v>18</v>
@@ -1335,10 +1292,10 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1352,10 +1309,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>104</v>
@@ -1369,10 +1326,10 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -1386,10 +1343,10 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -1403,10 +1360,10 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1420,10 +1377,10 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E45">
         <v>43</v>
@@ -1437,10 +1394,10 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1454,10 +1411,10 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E47">
         <v>3</v>
@@ -1471,10 +1428,10 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1488,10 +1445,10 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E49">
         <v>13</v>
@@ -1505,10 +1462,10 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E50">
         <v>3</v>
@@ -1522,10 +1479,10 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E51">
         <v>4</v>
@@ -1539,10 +1496,10 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E52">
         <v>34</v>
@@ -1556,10 +1513,10 @@
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E53">
         <v>6</v>
@@ -1573,10 +1530,10 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -1590,10 +1547,10 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -1607,10 +1564,10 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E56">
         <v>12</v>
@@ -1624,10 +1581,10 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -1641,10 +1598,10 @@
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E58">
         <v>35</v>
@@ -1658,10 +1615,10 @@
         <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E59">
         <v>57</v>
@@ -1675,10 +1632,10 @@
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E60">
         <v>2</v>
@@ -1692,10 +1649,10 @@
         <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E61">
         <v>15</v>
@@ -1709,10 +1666,10 @@
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -1726,10 +1683,10 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E63">
         <v>46</v>
@@ -1743,10 +1700,10 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -1760,10 +1717,10 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E65">
         <v>30</v>
@@ -1777,10 +1734,10 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E66">
         <v>5</v>
@@ -1794,10 +1751,10 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>52</v>
@@ -1811,10 +1768,10 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E68">
         <v>7</v>
@@ -1828,10 +1785,10 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E69">
         <v>5</v>
@@ -1845,10 +1802,10 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E70">
         <v>89</v>
@@ -1862,10 +1819,10 @@
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E71">
         <v>10</v>
@@ -1879,10 +1836,10 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D72" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E72">
         <v>6</v>
@@ -1896,10 +1853,10 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E73">
         <v>48</v>
@@ -1913,10 +1870,10 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E74">
         <v>32</v>
@@ -1930,10 +1887,10 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E75">
         <v>7</v>
@@ -1947,10 +1904,10 @@
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E76">
         <v>10</v>
@@ -1964,10 +1921,10 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -1981,10 +1938,10 @@
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -1998,10 +1955,10 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E79">
         <v>65</v>
@@ -2015,10 +1972,10 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E80">
         <v>10</v>
@@ -2032,10 +1989,10 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E81">
         <v>5</v>
@@ -2049,10 +2006,10 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E82">
         <v>41</v>
@@ -2066,10 +2023,10 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -2083,10 +2040,10 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D84" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E84">
         <v>3</v>
@@ -2100,10 +2057,10 @@
         <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E85">
         <v>24</v>
@@ -2117,10 +2074,10 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E86">
         <v>2</v>
@@ -2134,10 +2091,10 @@
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E87">
         <v>56</v>
@@ -2151,10 +2108,10 @@
         <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E88">
         <v>4</v>
@@ -2168,10 +2125,10 @@
         <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E89">
         <v>11</v>
@@ -2185,10 +2142,10 @@
         <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E90">
         <v>2</v>
@@ -2202,10 +2159,10 @@
         <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E91">
         <v>4</v>
@@ -2219,10 +2176,10 @@
         <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E92">
         <v>3</v>
@@ -2236,10 +2193,10 @@
         <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E93">
         <v>53</v>
@@ -2253,10 +2210,10 @@
         <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D94" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E94">
         <v>7</v>
@@ -2270,10 +2227,10 @@
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E95">
         <v>5</v>
@@ -2287,10 +2244,10 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E96">
         <v>72</v>
@@ -2304,10 +2261,10 @@
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E97">
         <v>6</v>
@@ -2321,10 +2278,10 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E98">
         <v>3</v>
@@ -2338,10 +2295,10 @@
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E99">
         <v>53</v>
@@ -2355,10 +2312,10 @@
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D100" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E100">
         <v>2</v>
@@ -2372,10 +2329,10 @@
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D101" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E101">
         <v>24</v>
@@ -2389,10 +2346,10 @@
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D102" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E102">
         <v>7</v>
@@ -2406,10 +2363,10 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D103" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E103">
         <v>6</v>
@@ -2423,10 +2380,10 @@
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D104" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -2440,10 +2397,10 @@
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D105" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -2457,10 +2414,10 @@
         <v>2</v>
       </c>
       <c r="C106" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E106">
         <v>3</v>
@@ -2474,10 +2431,10 @@
         <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E107">
         <v>4</v>
@@ -2491,16 +2448,10 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
+        <v>3</v>
+      </c>
+      <c r="F108" t="s">
         <v>10</v>
-      </c>
-      <c r="D108" t="s">
-        <v>21</v>
-      </c>
-      <c r="E108" t="s">
-        <v>21</v>
-      </c>
-      <c r="F108" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
@@ -2511,10 +2462,10 @@
         <v>2</v>
       </c>
       <c r="C109" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D109" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E109">
         <v>10</v>
@@ -2528,10 +2479,10 @@
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -2545,10 +2496,10 @@
         <v>2</v>
       </c>
       <c r="C111" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E111">
         <v>3</v>
@@ -2562,10 +2513,10 @@
         <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -2579,10 +2530,10 @@
         <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E113">
         <v>1</v>
@@ -2596,10 +2547,10 @@
         <v>3</v>
       </c>
       <c r="C114" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E114">
         <v>1</v>
@@ -2613,10 +2564,10 @@
         <v>3</v>
       </c>
       <c r="C115" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E115">
         <v>113</v>
@@ -2630,10 +2581,10 @@
         <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D116" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E116">
         <v>10</v>
@@ -2647,10 +2598,10 @@
         <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D117" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E117">
         <v>43</v>
@@ -2664,10 +2615,10 @@
         <v>3</v>
       </c>
       <c r="C118" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E118">
         <v>52</v>
@@ -2681,10 +2632,10 @@
         <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E119">
         <v>2</v>
@@ -2698,10 +2649,10 @@
         <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -2715,10 +2666,10 @@
         <v>4</v>
       </c>
       <c r="C121" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D121" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E121">
         <v>17</v>
@@ -2732,10 +2683,10 @@
         <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D122" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -2749,10 +2700,10 @@
         <v>4</v>
       </c>
       <c r="C123" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D123" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E123">
         <v>2</v>
@@ -2766,10 +2717,10 @@
         <v>4</v>
       </c>
       <c r="C124" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E124">
         <v>2</v>
@@ -2783,10 +2734,10 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D125" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E125">
         <v>3</v>
@@ -2800,10 +2751,10 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D126" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E126">
         <v>1</v>
@@ -2817,10 +2768,10 @@
         <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D127" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E127">
         <v>1</v>
@@ -2834,10 +2785,10 @@
         <v>5</v>
       </c>
       <c r="C128" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D128" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E128">
         <v>107</v>
@@ -2851,10 +2802,10 @@
         <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D129" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E129">
         <v>26</v>
@@ -2868,16 +2819,16 @@
         <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E130">
         <v>1</v>
       </c>
       <c r="F130" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
@@ -2888,10 +2839,10 @@
         <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E131">
         <v>44</v>
@@ -2905,16 +2856,16 @@
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E132">
         <v>1</v>
       </c>
       <c r="F132" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
@@ -2925,10 +2876,10 @@
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E133">
         <v>48</v>
@@ -2942,10 +2893,10 @@
         <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D134" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E134">
         <v>3</v>
@@ -2959,10 +2910,10 @@
         <v>1</v>
       </c>
       <c r="C135" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E135">
         <v>24</v>
@@ -2976,10 +2927,10 @@
         <v>1</v>
       </c>
       <c r="C136" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D136" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E136">
         <v>14</v>
@@ -2993,16 +2944,10 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>17</v>
-      </c>
-      <c r="D137" t="s">
-        <v>21</v>
-      </c>
-      <c r="E137" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F137" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
@@ -3013,10 +2958,10 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -3030,16 +2975,10 @@
         <v>2</v>
       </c>
       <c r="C139" t="s">
-        <v>10</v>
-      </c>
-      <c r="D139" t="s">
-        <v>21</v>
-      </c>
-      <c r="E139" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F139" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
@@ -3050,10 +2989,10 @@
         <v>2</v>
       </c>
       <c r="C140" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D140" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E140">
         <v>26</v>
@@ -3067,10 +3006,10 @@
         <v>2</v>
       </c>
       <c r="C141" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D141" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E141">
         <v>2</v>
@@ -3084,16 +3023,16 @@
         <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E142">
         <v>1</v>
       </c>
       <c r="F142" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
@@ -3104,10 +3043,10 @@
         <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D143" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E143">
         <v>70</v>
@@ -3121,10 +3060,10 @@
         <v>3</v>
       </c>
       <c r="C144" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D144" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E144">
         <v>2</v>
@@ -3138,10 +3077,10 @@
         <v>3</v>
       </c>
       <c r="C145" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D145" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E145">
         <v>30</v>
@@ -3155,10 +3094,10 @@
         <v>3</v>
       </c>
       <c r="C146" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D146" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E146">
         <v>70</v>
@@ -3172,10 +3111,10 @@
         <v>4</v>
       </c>
       <c r="C147" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D147" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E147">
         <v>8</v>
@@ -3189,10 +3128,10 @@
         <v>4</v>
       </c>
       <c r="C148" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D148" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E148">
         <v>17</v>
@@ -3206,10 +3145,10 @@
         <v>4</v>
       </c>
       <c r="C149" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D149" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -3223,10 +3162,10 @@
         <v>4</v>
       </c>
       <c r="C150" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D150" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E150">
         <v>3</v>
@@ -3240,10 +3179,10 @@
         <v>4</v>
       </c>
       <c r="C151" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D151" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E151">
         <v>1</v>
@@ -3257,10 +3196,10 @@
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D152" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E152">
         <v>1</v>
@@ -3274,10 +3213,10 @@
         <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D153" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E153">
         <v>1</v>
@@ -3291,10 +3230,10 @@
         <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D154" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E154">
         <v>22</v>
@@ -3308,10 +3247,10 @@
         <v>5</v>
       </c>
       <c r="C155" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D155" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E155">
         <v>102</v>
@@ -3325,10 +3264,10 @@
         <v>5</v>
       </c>
       <c r="C156" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D156" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E156">
         <v>7</v>
@@ -3342,10 +3281,10 @@
         <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D157" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E157">
         <v>123</v>
@@ -3359,10 +3298,10 @@
         <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E158">
         <v>1</v>
@@ -3376,16 +3315,10 @@
         <v>1</v>
       </c>
       <c r="C159" t="s">
+        <v>3</v>
+      </c>
+      <c r="F159" t="s">
         <v>10</v>
-      </c>
-      <c r="D159" t="s">
-        <v>21</v>
-      </c>
-      <c r="E159" t="s">
-        <v>21</v>
-      </c>
-      <c r="F159" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
@@ -3396,16 +3329,10 @@
         <v>1</v>
       </c>
       <c r="C160" t="s">
-        <v>13</v>
-      </c>
-      <c r="D160" t="s">
-        <v>21</v>
-      </c>
-      <c r="E160" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F160" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
@@ -3416,16 +3343,10 @@
         <v>1</v>
       </c>
       <c r="C161" t="s">
-        <v>17</v>
-      </c>
-      <c r="D161" t="s">
-        <v>21</v>
-      </c>
-      <c r="E161" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F161" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.35">
@@ -3436,16 +3357,12 @@
         <v>2</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
       <c r="F162" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.35">
@@ -3456,16 +3373,12 @@
         <v>2</v>
       </c>
       <c r="C163" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
@@ -3476,16 +3389,12 @@
         <v>2</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
       <c r="F164" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
@@ -3496,16 +3405,10 @@
         <v>2</v>
       </c>
       <c r="C165" t="s">
-        <v>17</v>
-      </c>
-      <c r="D165" t="s">
-        <v>21</v>
-      </c>
-      <c r="E165" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F165" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
@@ -3516,16 +3419,12 @@
         <v>3</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
       <c r="F166" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
@@ -3536,10 +3435,10 @@
         <v>3</v>
       </c>
       <c r="C167" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D167" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E167">
         <v>1</v>
@@ -3553,10 +3452,10 @@
         <v>3</v>
       </c>
       <c r="C168" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D168" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -3570,10 +3469,10 @@
         <v>3</v>
       </c>
       <c r="C169" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D169" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E169">
         <v>1</v>
@@ -3587,16 +3486,12 @@
         <v>4</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
       <c r="F170" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
@@ -3607,10 +3502,10 @@
         <v>4</v>
       </c>
       <c r="C171" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D171" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -3624,10 +3519,10 @@
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D172" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E172">
         <v>5</v>
@@ -3641,10 +3536,10 @@
         <v>4</v>
       </c>
       <c r="C173" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D173" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E173">
         <v>2</v>
@@ -3658,10 +3553,10 @@
         <v>4</v>
       </c>
       <c r="C174" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D174" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E174">
         <v>1</v>
@@ -3675,16 +3570,10 @@
         <v>5</v>
       </c>
       <c r="C175" t="s">
-        <v>6</v>
-      </c>
-      <c r="D175" t="s">
-        <v>21</v>
-      </c>
-      <c r="E175" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F175" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
@@ -3695,10 +3584,10 @@
         <v>5</v>
       </c>
       <c r="C176" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D176" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E176">
         <v>3</v>
@@ -3712,10 +3601,10 @@
         <v>5</v>
       </c>
       <c r="C177" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D177" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -3729,10 +3618,10 @@
         <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D178" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E178">
         <v>1</v>
@@ -3746,10 +3635,10 @@
         <v>5</v>
       </c>
       <c r="C179" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D179" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E179">
         <v>1</v>
@@ -3763,10 +3652,10 @@
         <v>5</v>
       </c>
       <c r="C180" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D180" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E180">
         <v>1</v>
@@ -3780,17 +3669,16 @@
         <v>5</v>
       </c>
       <c r="C181" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D181" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E181">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="L148" xr:uid="{639A35DF-5BDC-4DDF-BDD3-A0B339D8BC07}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>